<commit_message>
updated with Supporting files features
</commit_message>
<xml_diff>
--- a/docs/SIA_stdzn_automtn_action_plans_v3.xlsx
+++ b/docs/SIA_stdzn_automtn_action_plans_v3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\29. Innovation\Sentiment Analysis\0. Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\29. Innovation\Sentiment Analysis\7.2 Github\sia_automation upload_external\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B49CE4DF-626D-45D7-9BAF-F8DB8DCE36F5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57725C28-6F63-4EA8-B2C0-EC55DC35C273}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{243D77BE-137A-40EE-932D-9091A538030F}"/>
   </bookViews>
@@ -1441,7 +1441,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1654,7 +1654,7 @@
   <dimension ref="A1:AO17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection sqref="A1:U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>